<commit_message>
Updated Jira API token
</commit_message>
<xml_diff>
--- a/Tx_HyperAutomation_Project/Config/TestData.xlsx
+++ b/Tx_HyperAutomation_Project/Config/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tx-Hyper-Automation\Tx_HyperAutomation_Project\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E31175-AF35-4303-9D70-A72F77507EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A7A1D3-0A9E-498D-A54C-49BFB8808224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="850" firstSheet="0" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="850" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="TestCases" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <x:si>
     <x:t>Status</x:t>
   </x:si>
@@ -267,70 +267,43 @@
     <x:t>Column2</x:t>
   </x:si>
   <x:si>
-    <x:t>Test execution for Desktop Scenario started 12/06/2022 17:47:10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Desktop Scenario ended 12/06/2022 17:47:34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario started 12/06/2022 17:47:34</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario ended 12/06/2022 17:48:24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon Invalid Scenario started 12/06/2022 17:48:24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon Invalid Scenario ended 12/06/2022 17:48:47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Android Multiple Scenario started 12/06/2022 17:48:47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Android Multiple Scenario ended 12/06/2022 17:49:46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Android Login_Logout Scenario started 12/06/2022 17:49:46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Android Login_Logout Scenario ended 12/06/2022 17:50:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Multiple Scenario started 12/06/2022 17:50:07</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Multiple Scenario ended 12/06/2022 17:51:51</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Login_Logout Scenario started 12/06/2022 17:51:51</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Login_Logout Scenario ended 12/06/2022 17:52:25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Invalid Scenario started 12/06/2022 17:52:25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for IOS Invalid Scenario ended 12/06/2022 17:53:06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest Fail Scenario started 12/06/2022 17:53:06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest Fail Scenario ended 12/06/2022 17:53:14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest  Pass Scenario started 12/06/2022 17:53:14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest  Pass Scenario ended 12/06/2022 17:53:15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for SAP Add to cart Scenario started 12/06/2022 17:53:15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for SAP Add to cart Scenario ended 12/06/2022 17:56:47</x:t>
+    <x:t>Test execution for Desktop Scenario started 12/13/2022 16:56:49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Desktop Scenario ended 12/13/2022 16:57:12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario started 12/13/2022 16:57:12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario ended 12/13/2022 16:57:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario started 12/13/2022 16:57:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario ended 12/13/2022 16:58:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flag status - disabled</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest Fail Scenario started 12/13/2022 16:58:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest Fail Scenario ended 12/13/2022 16:58:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario started 12/13/2022 16:58:17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario ended 12/13/2022 16:58:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario started 12/13/2022 16:58:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario ended 12/13/2022 17:01:49</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -402,9 +375,8 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="20">
+  <x:cellStyleXfs count="30">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -459,8 +431,41 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="17">
+  <x:cellXfs count="16">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,8 +475,7 @@
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <x:xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -505,8 +509,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="2">
-    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -789,152 +792,152 @@
   </x:sheetPr>
   <x:dimension ref="A1:C12"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
+    <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="B16" sqref="B16 B16:B16"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="16.672344" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="32.344687" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="5.855469" style="9" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="105.140625" style="9" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="26.570312" style="9" customWidth="1"/>
-    <x:col min="4" max="4" width="8.855469" style="9" customWidth="1"/>
+    <x:col min="1" max="1" width="6.140625" style="8" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="105.140625" style="8" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="26.570312" style="8" customWidth="1"/>
+    <x:col min="4" max="4" width="8.855469" style="8" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="10" t="s">
+      <x:c r="A1" s="9" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="9" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="9" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="b">
+      <x:c r="A2" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="b">
+      <x:c r="A3" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C3" s="9" t="s">
+      <x:c r="C3" s="8" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="9" t="b">
+      <x:c r="A4" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B4" s="9" t="s">
+      <x:c r="B4" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C4" s="9" t="s">
+      <x:c r="C4" s="8" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="9" t="b">
+      <x:c r="A5" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B5" s="8" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C5" s="8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B6" s="8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C6" s="8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B7" s="8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C7" s="8" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B8" s="8" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C8" s="8" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="8" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C9" s="8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B5" s="9" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C5" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="9" t="b">
+      <x:c r="B10" s="8" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C10" s="8" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B6" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C6" s="9" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="9" t="b">
+      <x:c r="B11" s="8" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C11" s="8" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B7" s="9" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C7" s="9" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B8" s="9" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C8" s="9" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B9" s="9" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C9" s="9" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B10" s="9" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C10" s="9" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B11" s="9" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C11" s="9" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B12" s="9" t="s">
+      <x:c r="B12" s="8" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C12" s="9" t="s">
+      <x:c r="C12" s="8" t="s">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4">
-      <x:c r="B16" s="9" t="s"/>
+      <x:c r="B16" s="8" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -958,51 +961,51 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
-    <x:col min="2" max="2" width="25" style="9" customWidth="1"/>
-    <x:col min="3" max="3" width="21.425781" style="9" customWidth="1"/>
-    <x:col min="4" max="4" width="14.140625" style="9" customWidth="1"/>
+    <x:col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
+    <x:col min="2" max="2" width="25" style="8" customWidth="1"/>
+    <x:col min="3" max="3" width="21.425781" style="8" customWidth="1"/>
+    <x:col min="4" max="4" width="14.140625" style="8" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="12" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="12" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="12" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="12" t="s">
         <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="12" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="B2" s="11" t="s">
+      <x:c r="B2" s="10" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C2" s="11" t="s">
+      <x:c r="C2" s="10" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="D2" s="9" t="s">
+      <x:c r="D2" s="8" t="s">
         <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="s">
+      <x:c r="A3" s="8" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId14"/>
+    <x:hyperlink ref="B2" r:id="rId13"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1025,51 +1028,51 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
-    <x:col min="2" max="2" width="14.425781" style="9" customWidth="1"/>
+    <x:col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
+    <x:col min="2" max="2" width="14.425781" style="8" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="14" t="s">
+    <x:row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="13" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="14" t="s">
+      <x:c r="B1" s="13" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C1" s="14" t="s">
+      <x:c r="C1" s="13" t="s">
         <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="b">
+      <x:c r="A2" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="b">
+      <x:c r="A3" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="C3" s="9" t="s">
+      <x:c r="C3" s="8" t="s">
         <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="9" t="b">
+      <x:c r="A4" s="8" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B4" s="9" t="s">
+      <x:c r="B4" s="8" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C4" s="9" t="s">
+      <x:c r="C4" s="8" t="s">
         <x:v>41</x:v>
       </x:c>
     </x:row>
@@ -1093,24 +1096,24 @@
       <x:selection activeCell="A3" sqref="A3 A3:A3"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="16.816875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="32.489219" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="76" style="9" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="9" style="9" customWidth="1"/>
+    <x:col min="1" max="1" width="76" style="8" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="9" style="8" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="9" t="s">
+      <x:c r="A1" s="8" t="s">
         <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="8" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="s">
+      <x:c r="A3" s="8" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
@@ -1137,72 +1140,72 @@
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="12" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="12" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="12" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="12" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="E1" s="13" t="s">
+      <x:c r="E1" s="12" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="12" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="G1" s="13" t="s">
+      <x:c r="G1" s="12" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="12" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="I1" s="13" t="s">
+      <x:c r="I1" s="12" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="J1" s="13" t="s">
+      <x:c r="J1" s="12" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="K1" s="13" t="s">
+      <x:c r="K1" s="12" t="s">
         <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="12" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="D2" s="12" t="s">
+      <x:c r="D2" s="11" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="E2" s="12" t="s">
+      <x:c r="E2" s="11" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="F2" s="15" t="s">
+      <x:c r="F2" s="14" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="G2" s="12" t="s">
+      <x:c r="G2" s="11" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="H2" s="12" t="s">
+      <x:c r="H2" s="11" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="I2" s="9" t="s">
+      <x:c r="I2" s="8" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="J2" s="12" t="s">
+      <x:c r="J2" s="11" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="K2" s="12" t="s">
+      <x:c r="K2" s="11" t="s">
         <x:v>60</x:v>
       </x:c>
     </x:row>
@@ -1229,58 +1232,58 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="5" width="9.140625" style="9" customWidth="1"/>
-    <x:col min="6" max="6" width="10.855469" style="9" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="5" width="9.140625" style="8" customWidth="1"/>
+    <x:col min="6" max="6" width="10.855469" style="8" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="9" t="s">
+      <x:c r="A1" s="8" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B1" s="9" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="C1" s="9" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="D1" s="9" t="s">
+      <x:c r="D1" s="8" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="E1" s="9" t="s">
+      <x:c r="E1" s="8" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="F1" s="9" t="s">
+      <x:c r="F1" s="8" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="G1" s="9" t="s">
+      <x:c r="G1" s="8" t="s">
         <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="8" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="D2" s="9" t="s">
+      <x:c r="D2" s="8" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="E2" s="9" t="s">
+      <x:c r="E2" s="8" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="F2" s="9" t="n">
+      <x:c r="F2" s="8" t="n">
         <x:v>1330019087</x:v>
       </x:c>
-      <x:c r="G2" s="16" t="s">
+      <x:c r="G2" s="15" t="s">
         <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
-      <x:c r="F11" s="9" t="s"/>
+      <x:c r="F11" s="8" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -1305,89 +1308,89 @@
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="12" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="12" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="12" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="12" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="E1" s="13" t="s">
+      <x:c r="E1" s="12" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="12" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="G1" s="13" t="s">
+      <x:c r="G1" s="12" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="12" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="I1" s="13" t="s">
+      <x:c r="I1" s="12" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="J1" s="13" t="s">
+      <x:c r="J1" s="12" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="K1" s="13" t="s">
+      <x:c r="K1" s="12" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="L1" s="13" t="s">
+      <x:c r="L1" s="12" t="s">
         <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="12" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="D2" s="12" t="s">
+      <x:c r="D2" s="11" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="E2" s="12" t="s">
+      <x:c r="E2" s="11" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="F2" s="15" t="s">
+      <x:c r="F2" s="14" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="G2" s="12" t="s">
+      <x:c r="G2" s="11" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="H2" s="12" t="s">
+      <x:c r="H2" s="11" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="I2" s="9" t="s">
+      <x:c r="I2" s="8" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="J2" s="12" t="s">
+      <x:c r="J2" s="11" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="K2" s="12" t="s">
+      <x:c r="K2" s="11" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="L2" s="12" t="s">
+      <x:c r="L2" s="11" t="s">
         <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="12" t="s">
+      <x:c r="A3" s="11" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="C3" s="9" t="s">
+      <x:c r="C3" s="8" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
@@ -1408,221 +1411,224 @@
   </x:sheetPr>
   <x:dimension ref="A1:E12"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D9" sqref="D9 D9:D9"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="B18" sqref="B18 B18:B18"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
-    <x:col min="2" max="2" width="85.425781" style="9" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="26.855469" style="9" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="67.140625" style="9" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
+    <x:col min="2" max="2" width="85.425781" style="8" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="26.855469" style="8" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="67.140625" style="8" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="9" t="s">
+      <x:c r="A1" s="8" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="9" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="9" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="9" t="s">
+      <x:c r="D1" s="8" t="s">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="E1" s="9" t="s">
+      <x:c r="E1" s="8" t="s">
         <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="b">
+      <x:c r="A2" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D2" s="9" t="s">
+      <x:c r="D2" s="8" t="s">
         <x:v>79</x:v>
       </x:c>
-      <x:c r="E2" s="9" t="s">
+      <x:c r="E2" s="8" t="s">
         <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="b">
+      <x:c r="A3" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C3" s="9" t="s">
+      <x:c r="C3" s="8" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D3" s="9" t="s">
+      <x:c r="D3" s="8" t="s">
         <x:v>81</x:v>
       </x:c>
-      <x:c r="E3" s="9" t="s">
+      <x:c r="E3" s="8" t="s">
         <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="9" t="b">
+      <x:c r="A4" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B4" s="9" t="s">
+      <x:c r="B4" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C4" s="9" t="s">
+      <x:c r="C4" s="8" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D4" s="9" t="s">
+      <x:c r="D4" s="8" t="s">
         <x:v>83</x:v>
       </x:c>
-      <x:c r="E4" s="9" t="s">
+      <x:c r="E4" s="8" t="s">
         <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="9" t="b">
+      <x:c r="A5" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B5" s="8" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C5" s="8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D5" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E5" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B6" s="8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C6" s="8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D6" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E6" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B7" s="8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C7" s="8" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D7" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E7" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B8" s="8" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C8" s="8" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D8" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E8" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="8" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="8" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C9" s="8" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D9" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="E9" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B5" s="9" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C5" s="9" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D5" s="9" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="E5" s="9" t="s">
+      <x:c r="B10" s="8" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C10" s="8" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D10" s="8" t="s">
         <x:v>86</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="9" t="b">
+      <x:c r="E10" s="8" t="s">
+        <x:v>87</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B6" s="9" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C6" s="9" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D6" s="9" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="E6" s="9" t="s">
+      <x:c r="B11" s="8" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C11" s="8" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D11" s="8" t="s">
         <x:v>88</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="9" t="b">
+      <x:c r="E11" s="8" t="s">
+        <x:v>89</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="8" t="b">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B7" s="9" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C7" s="9" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D7" s="9" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="E7" s="9" t="s">
+      <x:c r="B12" s="8" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C12" s="8" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D12" s="8" t="s">
         <x:v>90</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B8" s="9" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C8" s="9" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="D8" s="9" t="s">
+      <x:c r="E12" s="8" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="E8" s="9" t="s">
-        <x:v>92</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B9" s="9" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C9" s="9" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D9" s="9" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="E9" s="9" t="s">
-        <x:v>94</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B10" s="9" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C10" s="9" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D10" s="9" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="E10" s="9" t="s">
-        <x:v>96</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B11" s="9" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C11" s="9" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D11" s="9" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="E11" s="9" t="s">
-        <x:v>98</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="9" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B12" s="9" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C12" s="9" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="D12" s="9" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="E12" s="9" t="s">
-        <x:v>100</x:v>
-      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5">
+      <x:c r="B18" s="8" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Updated API key for Jira
</commit_message>
<xml_diff>
--- a/Tx_HyperAutomation_Project/Config/TestData.xlsx
+++ b/Tx_HyperAutomation_Project/Config/TestData.xlsx
@@ -267,43 +267,43 @@
     <x:t>Column2</x:t>
   </x:si>
   <x:si>
-    <x:t>Test execution for Desktop Scenario started 12/13/2022 16:56:49</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Desktop Scenario ended 12/13/2022 16:57:12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario started 12/13/2022 16:57:12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario ended 12/13/2022 16:57:50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon Invalid Scenario started 12/13/2022 16:57:50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon Invalid Scenario ended 12/13/2022 16:58:08</x:t>
+    <x:t>Test execution for Desktop Scenario started 12/14/2022 17:44:50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Desktop Scenario ended 12/14/2022 17:45:12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario started 12/14/2022 17:45:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario ended 12/14/2022 17:45:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario started 12/14/2022 17:45:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario ended 12/14/2022 17:46:15</x:t>
   </x:si>
   <x:si>
     <x:t>Flag status - disabled</x:t>
   </x:si>
   <x:si>
-    <x:t>Test execution for ApiTest Fail Scenario started 12/13/2022 16:58:08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest Fail Scenario ended 12/13/2022 16:58:17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest  Pass Scenario started 12/13/2022 16:58:17</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for ApiTest  Pass Scenario ended 12/13/2022 16:58:19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for SAP Add to cart Scenario started 12/13/2022 16:58:19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for SAP Add to cart Scenario ended 12/13/2022 17:01:49</x:t>
+    <x:t>Test execution for ApiTest Fail Scenario started 12/14/2022 17:46:16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest Fail Scenario ended 12/14/2022 17:46:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario started 12/14/2022 17:46:25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario ended 12/14/2022 17:46:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario started 12/14/2022 17:46:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario ended 12/14/2022 17:50:01</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -375,7 +375,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="30">
+  <x:cellStyleXfs count="73">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -399,6 +399,135 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="17" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -796,7 +925,7 @@
       <x:selection activeCell="B16" sqref="B16 B16:B16"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="32.344687" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="62.901562" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="6.140625" style="8" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="105.140625" style="8" bestFit="1" customWidth="1"/>
@@ -1005,7 +1134,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="B2" r:id="rId13"/>
+    <x:hyperlink ref="B2" r:id="rId14"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1096,7 +1225,7 @@
       <x:selection activeCell="A3" sqref="A3 A3:A3"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="32.489219" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultColWidth="63.046094" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="76" style="8" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="9" style="8" customWidth="1"/>

</xml_diff>